<commit_message>
Modification document du groupe
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="UserStories" sheetId="1" r:id="rId1"/>
-    <sheet name="BurndownChart1" sheetId="2" r:id="rId2"/>
-    <sheet name="BurndownChart2" sheetId="4" r:id="rId3"/>
+    <sheet name="UserStories-Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="BurndownChart1-Sprint1" sheetId="2" r:id="rId2"/>
+    <sheet name="BurndownChart2-Sprint2" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -381,7 +381,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurndownChart1!$E$12</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$E$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -392,7 +392,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>BurndownChart1!$I$1:$O$1</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$I$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -421,7 +421,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurndownChart1!$I$12:$O$12</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$I$12:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -435,7 +435,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurndownChart1!$E$13</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$E$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -446,7 +446,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>BurndownChart1!$I$13:$O$13</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$I$13:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -580,7 +580,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurndownChart2!$E$12</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$E$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -591,7 +591,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>BurndownChart2!$I$1:$O$1</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$I$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -620,7 +620,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurndownChart2!$I$12:$O$12</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$I$12:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -634,7 +634,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurndownChart2!$E$13</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$E$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -645,7 +645,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>BurndownChart2!$I$13:$O$13</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$I$13:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>

</xml_diff>

<commit_message>
Fusion du document de groupe avec les stories
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -4,22 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories-Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="BurndownChart1-Sprint1" sheetId="2" r:id="rId2"/>
     <sheet name="BurndownChart2-Sprint2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
   <si>
     <t>Nom</t>
   </si>
@@ -102,7 +99,136 @@
     <t>Page 2</t>
   </si>
   <si>
-    <t>Page 1</t>
+    <t>US001</t>
+  </si>
+  <si>
+    <t>Connexion a la base de donnée</t>
+  </si>
+  <si>
+    <t>US002</t>
+  </si>
+  <si>
+    <t>Menu principal</t>
+  </si>
+  <si>
+    <t>US003</t>
+  </si>
+  <si>
+    <t>Afiche la liste des cabanes</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur , je veux pouvoir me connecter a une base de donnée MySql avec un application C#</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux avoir un menu principal (Une Fenetre) qui me permet d'accéder aux pages de mon application via des bouttons. Les bountons seront : Liste des Cabanes, Ajouter une Cabane, Listes des contacts, Ajouter un Contact, Affecter  un Contact</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux depuis le menu principal en US002 pouvoir ouvrir une fenetre qui affiche la liste des cabanes avec les informations suivante : Nom Cabane, Douche (Oui/Non)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Story Points : </t>
+  </si>
+  <si>
+    <t>US004</t>
+  </si>
+  <si>
+    <t>Affiche une cabane détaillée</t>
+  </si>
+  <si>
+    <t>US005</t>
+  </si>
+  <si>
+    <t>Possibilité Modifier / Supprimer une cabane</t>
+  </si>
+  <si>
+    <t>US006</t>
+  </si>
+  <si>
+    <t>Modifier une cabane</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux que en cliquant sur le nom de la cabane dans la liste en US003, une fenetre s'ouvre et m'affiche tous les détails(Photo, Nom, Nombre de places, ...) de cette cabane dans des labels et avec une description du détail</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux que depuis la fenetre en US004 avoir l'accès a deux fenetres (boutons)  qui permetront de modifier et supprimer une cabane</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux pouvoir modifier la cabane de US005 dans une fenetre qui contient les composants les plus aptes à la modification du type d'informations (Text, Liste, Date, Boolean,...)</t>
+  </si>
+  <si>
+    <t>US007</t>
+  </si>
+  <si>
+    <t>Supprimer une cabane</t>
+  </si>
+  <si>
+    <t>US008</t>
+  </si>
+  <si>
+    <t>Rechercher une cabane</t>
+  </si>
+  <si>
+    <t>US009</t>
+  </si>
+  <si>
+    <t>Mise a jour Liste des Cabanes</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux pouvoir supprimer la cabane en US004 en restant sur la meme page. Un message de confirmation apparait et doit etre accepter pour supprimer la cabane</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur,  je veux pouvoir rechercher une cabane en tapant son nom dans un edit sur la fenetre Liste des cabanes en US003</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux que la liste en US003 se mette à jour en cas d'une recherche en US008</t>
+  </si>
+  <si>
+    <t>US010</t>
+  </si>
+  <si>
+    <t>Créer une cabane</t>
+  </si>
+  <si>
+    <t>US011</t>
+  </si>
+  <si>
+    <t>Liste des contacts</t>
+  </si>
+  <si>
+    <t>US012</t>
+  </si>
+  <si>
+    <t>Modifier un contact</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux pouvoir créer une cabane sur une nouvelle fenetre accessible depuis le menu en US002 Toutes les inofrmations sont obligatoire</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux depuis le menu principal en US002 pouvoir ouvrir une fenetre qui affiche la liste des contacts avec toutes les informations</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur je veux pouvoir modifier un contact dans une nouvelle fenetre depuis la liste des contacts en US011</t>
+  </si>
+  <si>
+    <t>US014</t>
+  </si>
+  <si>
+    <t>Supprimer un contact</t>
+  </si>
+  <si>
+    <t>US015</t>
+  </si>
+  <si>
+    <t>Créer un contact</t>
+  </si>
+  <si>
+    <t>US016</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur, je veux pouvoir supprimer un contact depuis la liste des conacts en US011.  Un message de confirmation apparait et doit etre accepter pour supprimer le contact</t>
+  </si>
+  <si>
+    <t>En tant qu'tilisateur, je veux pouvoir créer un nouveau contact sur une nouvelle fenetre accessible depuis le menu en US002</t>
   </si>
 </sst>
 </file>
@@ -159,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +304,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -258,24 +396,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -291,6 +503,22 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -298,14 +526,25 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,11 +704,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90783232"/>
-        <c:axId val="47426368"/>
+        <c:axId val="100689408"/>
+        <c:axId val="100968128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90783232"/>
+        <c:axId val="100689408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,7 +718,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47426368"/>
+        <c:crossAx val="100968128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -487,7 +726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47426368"/>
+        <c:axId val="100968128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,7 +736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="90783232"/>
+        <c:crossAx val="100689408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -664,11 +903,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90782720"/>
-        <c:axId val="96148224"/>
+        <c:axId val="96361984"/>
+        <c:axId val="89887808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90782720"/>
+        <c:axId val="96361984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +917,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96148224"/>
+        <c:crossAx val="89887808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -686,7 +925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96148224"/>
+        <c:axId val="89887808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +935,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="90782720"/>
+        <c:crossAx val="96361984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -790,66 +1029,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Feuil1"/>
-      <sheetName val="Feuil2"/>
-      <sheetName val="Feuil3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="F6" t="str">
-            <v>Start</v>
-          </cell>
-          <cell r="G6" t="str">
-            <v>Day 1</v>
-          </cell>
-          <cell r="H6" t="str">
-            <v>Day 2</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>Day 3</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="F17">
-            <v>51</v>
-          </cell>
-          <cell r="G17">
-            <v>34</v>
-          </cell>
-          <cell r="H17">
-            <v>17</v>
-          </cell>
-          <cell r="I17">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="F18">
-            <v>51</v>
-          </cell>
-          <cell r="G18">
-            <v>26</v>
-          </cell>
-          <cell r="H18">
-            <v>16</v>
-          </cell>
-          <cell r="I18">
-            <v>10</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1139,57 +1318,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D4" s="15"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="17"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1199,8 +1412,9 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1210,8 +1424,9 @@
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1221,17 +1436,263 @@
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
-    </row>
+      <c r="C11" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="B12" s="28"/>
+      <c r="C12" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="28"/>
+      <c r="I12" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="30"/>
+      <c r="C13" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="30"/>
+      <c r="C17" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="28"/>
+      <c r="C20" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="28"/>
+      <c r="I20" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="30"/>
+      <c r="C21" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B24" s="28"/>
+      <c r="C24" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="28"/>
+      <c r="F24" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="28"/>
+      <c r="I24" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="30"/>
+      <c r="C25" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B28" s="28"/>
+      <c r="C28" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="28"/>
+      <c r="I28" s="29"/>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="30"/>
+      <c r="C29" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="30"/>
+      <c r="I29" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A35:C35"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
@@ -1246,7 +1707,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,83 +1718,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="16">
+      <c r="J1" s="10">
         <v>41942</v>
       </c>
-      <c r="K1" s="16">
+      <c r="K1" s="10">
         <v>41949</v>
       </c>
-      <c r="L1" s="16">
+      <c r="L1" s="10">
         <v>41956</v>
       </c>
-      <c r="M1" s="16">
+      <c r="M1" s="10">
         <v>41963</v>
       </c>
-      <c r="N1" s="16">
+      <c r="N1" s="10">
         <v>41970</v>
       </c>
-      <c r="O1" s="17">
+      <c r="O1" s="11">
         <v>41977</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="6"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="6"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1342,21 +1803,21 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1365,21 +1826,21 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="6"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1392,17 +1853,17 @@
         <v>10</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="6"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1415,17 +1876,17 @@
         <v>10</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="6"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1438,115 +1899,115 @@
         <v>10</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="6"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="6"/>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="6"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="6"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="12"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1567,7 +2028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:C35"/>
     </sheetView>
   </sheetViews>
@@ -1579,83 +2040,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="16">
+      <c r="J1" s="10">
         <v>41942</v>
       </c>
-      <c r="K1" s="16">
+      <c r="K1" s="10">
         <v>41949</v>
       </c>
-      <c r="L1" s="16">
+      <c r="L1" s="10">
         <v>41956</v>
       </c>
-      <c r="M1" s="16">
+      <c r="M1" s="10">
         <v>41963</v>
       </c>
-      <c r="N1" s="16">
+      <c r="N1" s="10">
         <v>41970</v>
       </c>
-      <c r="O1" s="17">
+      <c r="O1" s="11">
         <v>41977</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="6"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="6"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1664,21 +2125,21 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1687,21 +2148,21 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="6"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1714,17 +2175,17 @@
         <v>10</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="6"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1737,17 +2198,17 @@
         <v>10</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="6"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1760,115 +2221,115 @@
         <v>10</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="6"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="6"/>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="6"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="7" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="6"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="12"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Ajout des story point
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270"/>
+    <workbookView xWindow="330" yWindow="360" windowWidth="24915" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories-Backlog" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
   <si>
     <t>Nom</t>
   </si>
@@ -229,6 +229,18 @@
   </si>
   <si>
     <t>En tant qu'tilisateur, je veux pouvoir créer un nouveau contact sur une nouvelle fenetre accessible depuis le menu en US002</t>
+  </si>
+  <si>
+    <t>Story Points : 2100</t>
+  </si>
+  <si>
+    <t>Story Points : 500</t>
+  </si>
+  <si>
+    <t>Story Points :  2100</t>
+  </si>
+  <si>
+    <t>Story Points : 1300</t>
   </si>
 </sst>
 </file>
@@ -509,23 +521,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -544,6 +539,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,11 +716,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100689408"/>
-        <c:axId val="100968128"/>
+        <c:axId val="66321408"/>
+        <c:axId val="31508160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100689408"/>
+        <c:axId val="66321408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +730,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100968128"/>
+        <c:crossAx val="31508160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -726,7 +738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100968128"/>
+        <c:axId val="31508160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,14 +748,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="100689408"/>
+        <c:crossAx val="66321408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -903,11 +914,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96361984"/>
-        <c:axId val="89887808"/>
+        <c:axId val="63360512"/>
+        <c:axId val="31510464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96361984"/>
+        <c:axId val="63360512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +928,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89887808"/>
+        <c:crossAx val="31510464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -925,7 +936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89887808"/>
+        <c:axId val="31510464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,14 +946,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="96361984"/>
+        <c:crossAx val="63360512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1320,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,11 +1345,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1351,22 +1361,22 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1375,15 +1385,15 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1392,15 +1402,15 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1450,243 +1460,243 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
+    <row r="11" spans="1:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="29" t="s">
+    <row r="12" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="29" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
-      <c r="C13" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31" t="s">
-        <v>36</v>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+    <row r="15" spans="1:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="H15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="C16" s="29" t="s">
+    <row r="16" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
-      <c r="C17" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="31" t="s">
-        <v>36</v>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+    <row r="19" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="C20" s="29" t="s">
+    <row r="20" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29" t="s">
+      <c r="H20" s="17"/>
+      <c r="I20" s="18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
-      <c r="C21" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="31" t="s">
-        <v>36</v>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="19"/>
+      <c r="I21" s="20" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
+    <row r="23" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="27" t="s">
+      <c r="I23" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
-      <c r="C24" s="29" t="s">
+    <row r="24" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="29" t="s">
+      <c r="H24" s="17"/>
+      <c r="I24" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="30"/>
-      <c r="C25" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31" t="s">
-        <v>36</v>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="19"/>
+      <c r="I25" s="20" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="26" t="s">
+    <row r="27" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="26" t="s">
+      <c r="H27" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="I27" s="27"/>
-    </row>
-    <row r="28" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
-      <c r="C28" s="29" t="s">
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29" t="s">
+      <c r="E28" s="17"/>
+      <c r="F28" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="30"/>
-      <c r="C29" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="19"/>
+      <c r="I29" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1718,11 +1728,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="1"/>
       <c r="E1" s="8" t="s">
         <v>20</v>
@@ -1803,10 +1813,10 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1826,10 +1836,10 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1929,11 +1939,11 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
@@ -1948,9 +1958,9 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -1965,15 +1975,15 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1988,11 +1998,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -2003,11 +2013,11 @@
       <c r="O13" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2040,11 +2050,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="1"/>
       <c r="E1" s="8" t="s">
         <v>20</v>
@@ -2125,10 +2135,10 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -2148,10 +2158,10 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2251,12 +2261,12 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="22"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -2270,10 +2280,10 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2287,15 +2297,15 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="18" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -2310,11 +2320,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -2325,11 +2335,11 @@
       <c r="O13" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Ajout des points de difficulté
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
   <si>
     <t>Nom</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Story Points : 1300</t>
+  </si>
+  <si>
+    <t>Technicien Team Leader</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -521,6 +524,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -544,8 +550,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1330,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,11 +1349,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1361,22 +1365,22 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1385,15 +1389,15 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1402,15 +1406,15 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1420,7 +1424,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -1461,251 +1465,277 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="18" t="s">
+      <c r="H12" s="20"/>
+      <c r="I12" s="21" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20" t="s">
+      <c r="B13" s="22">
+        <v>34</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20" t="s">
+      <c r="E13" s="22">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20" t="s">
+      <c r="H13" s="22">
+        <v>55</v>
+      </c>
+      <c r="I13" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="20"/>
+      <c r="F16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18" t="s">
+      <c r="H16" s="20"/>
+      <c r="I16" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20" t="s">
+      <c r="B17" s="22">
+        <v>21</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20" t="s">
+      <c r="E17" s="22">
+        <v>2</v>
+      </c>
+      <c r="F17" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20" t="s">
+      <c r="H17" s="22">
+        <v>34</v>
+      </c>
+      <c r="I17" s="23" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18" t="s">
+      <c r="H20" s="20"/>
+      <c r="I20" s="21" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="s">
+      <c r="B21" s="22">
+        <v>21</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20" t="s">
+      <c r="E21" s="22">
+        <v>89</v>
+      </c>
+      <c r="F21" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20" t="s">
+      <c r="H21" s="22">
+        <v>13</v>
+      </c>
+      <c r="I21" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="18" t="s">
+      <c r="H24" s="20"/>
+      <c r="I24" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20" t="s">
+      <c r="B25" s="22">
+        <v>34</v>
+      </c>
+      <c r="C25" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20" t="s">
+      <c r="E25" s="22">
+        <v>55</v>
+      </c>
+      <c r="F25" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20" t="s">
+      <c r="H25" s="22">
+        <v>34</v>
+      </c>
+      <c r="I25" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="H27" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="I27" s="16"/>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18" t="s">
+      <c r="E28" s="20"/>
+      <c r="F28" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="18"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="22">
+        <v>21</v>
+      </c>
+      <c r="C29" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="20" t="s">
+      <c r="E29" s="22">
+        <v>34</v>
+      </c>
+      <c r="F29" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20" t="s">
+      <c r="H29" s="22"/>
+      <c r="I29" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1728,11 +1758,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="1"/>
       <c r="E1" s="8" t="s">
         <v>20</v>
@@ -1813,10 +1843,10 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1836,10 +1866,10 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1939,11 +1969,11 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
@@ -1958,9 +1988,9 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -1975,15 +2005,15 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1998,11 +2028,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -2013,11 +2043,11 @@
       <c r="O13" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2050,11 +2080,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="1"/>
       <c r="E1" s="8" t="s">
         <v>20</v>
@@ -2135,10 +2165,10 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -2158,10 +2188,10 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2261,12 +2291,12 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="29"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -2280,10 +2310,10 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="29"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2297,15 +2327,15 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="25" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -2320,11 +2350,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -2335,11 +2365,11 @@
       <c r="O13" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Mise à jour progression du projet.
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
   <si>
     <t>Nom</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -571,6 +574,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,9 +592,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -762,6 +765,12 @@
                 <c:pt idx="1">
                   <c:v>14400</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>14400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6300</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -777,11 +786,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101638144"/>
-        <c:axId val="90806464"/>
+        <c:axId val="122552320"/>
+        <c:axId val="85694656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101638144"/>
+        <c:axId val="122552320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,7 +800,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90806464"/>
+        <c:crossAx val="85694656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -799,7 +808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90806464"/>
+        <c:axId val="85694656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="101638144"/>
+        <c:crossAx val="122552320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -976,11 +985,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96839168"/>
-        <c:axId val="101794368"/>
+        <c:axId val="93242880"/>
+        <c:axId val="102777408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96839168"/>
+        <c:axId val="93242880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +999,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101794368"/>
+        <c:crossAx val="102777408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +1007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101794368"/>
+        <c:axId val="102777408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,13 +1017,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="96839168"/>
+        <c:crossAx val="93242880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1392,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -1407,11 +1417,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1805,7 +1815,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="P7" sqref="P7:R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1818,11 +1828,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
       <c r="E1" s="24" t="s">
         <v>20</v>
       </c>
@@ -1880,7 +1890,9 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
@@ -1902,7 +1914,9 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="4"/>
@@ -1914,10 +1928,10 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="25" t="s">
         <v>31</v>
       </c>
@@ -1933,7 +1947,9 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="4"/>
@@ -1945,10 +1961,10 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="25" t="s">
         <v>37</v>
       </c>
@@ -2079,17 +2095,19 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="4"/>
       <c r="E10" s="25" t="s">
         <v>50</v>
@@ -2106,20 +2124,22 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="E11" s="31" t="s">
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="E11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="1">
         <f>SUM(H2:H10)</f>
         <v>14900</v>
@@ -2148,11 +2168,11 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5">
         <v>14900</v>
@@ -2161,8 +2181,12 @@
         <f>I11-H3</f>
         <v>14400</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="K12" s="5">
+        <v>14400</v>
+      </c>
+      <c r="L12" s="5">
+        <v>6300</v>
+      </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="6"/>
@@ -2182,14 +2206,14 @@
         <f>SUM(G2:G10)</f>
         <v>270</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="27" t="s">
         <v>75</v>
       </c>
       <c r="J14" s="3">
         <f>SUM(H11)</f>
         <v>14900</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="27" t="s">
         <v>76</v>
       </c>
       <c r="L14" s="3">
@@ -2201,11 +2225,11 @@
       <c r="O14" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="28"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2239,11 +2263,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="1"/>
       <c r="E1" s="8" t="s">
         <v>20</v>
@@ -2324,10 +2348,10 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -2347,10 +2371,10 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2450,12 +2474,12 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="36"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -2469,10 +2493,10 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2486,15 +2510,15 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="31" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -2509,11 +2533,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -2524,11 +2548,11 @@
       <c r="O13" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
MAJ Document pour retro
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4065" yWindow="270" windowWidth="24915" windowHeight="12270" activeTab="1"/>
+    <workbookView xWindow="-4065" yWindow="270" windowWidth="24915" windowHeight="12270" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories-Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="BurndownChart1-Sprint1" sheetId="5" r:id="rId2"/>
-    <sheet name="BurndownChart2-Sprint2" sheetId="4" r:id="rId3"/>
+    <sheet name="BurndownChart2-Sprint2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
   <si>
     <t>Nom</t>
   </si>
@@ -87,15 +87,9 @@
     <t>30 octobre 2014</t>
   </si>
   <si>
-    <t>6 novembre 2014</t>
-  </si>
-  <si>
     <t>Team C</t>
   </si>
   <si>
-    <t>Page 3</t>
-  </si>
-  <si>
     <t>Page 2</t>
   </si>
   <si>
@@ -250,13 +244,16 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>27 novembre 2014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,14 +294,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -338,22 +327,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -512,32 +490,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -547,32 +551,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,17 +583,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,8 +682,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="1.3666969711990809E-2"/>
-          <c:y val="0.22452807027717767"/>
-          <c:w val="0.98120791664601259"/>
+          <c:y val="0.19670634611406487"/>
+          <c:w val="0.92568585219105015"/>
           <c:h val="0.70501341894454117"/>
         </c:manualLayout>
       </c:layout>
@@ -680,9 +706,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'BurndownChart1-Sprint1'!$I$1:$O$1</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$I$1:$M$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Start</c:v>
                 </c:pt>
@@ -697,41 +723,29 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>27.11.2014</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>04.12.2014</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.12.2014</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BurndownChart1-Sprint1'!$I$11:$O$11</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$I$11:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>14900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12416.66666666667</c:v>
+                  <c:v>11175</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9933.3333333332994</c:v>
+                  <c:v>7450</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7450</c:v>
+                  <c:v>3725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4966.6666666666597</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2483.3333333333298</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -753,12 +767,35 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'BurndownChart1-Sprint1'!$I$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>06.11.2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.11.2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.11.2014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.11.2014</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BurndownChart1-Sprint1'!$I$12:$O$12</c:f>
+              <c:f>'BurndownChart1-Sprint1'!$I$12:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>14900</c:v>
                 </c:pt>
@@ -769,6 +806,9 @@
                   <c:v>14400</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4200</c:v>
                 </c:pt>
               </c:numCache>
@@ -786,11 +826,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97525760"/>
-        <c:axId val="84580544"/>
+        <c:axId val="126554112"/>
+        <c:axId val="95000768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97525760"/>
+        <c:axId val="126554112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +840,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84580544"/>
+        <c:crossAx val="95000768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -808,7 +848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84580544"/>
+        <c:axId val="95000768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="97525760"/>
+        <c:crossAx val="126554112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -888,8 +928,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="1.3666969711990809E-2"/>
-          <c:y val="0.22452807027717767"/>
-          <c:w val="0.98120791664601259"/>
+          <c:y val="0.19670634611406487"/>
+          <c:w val="0.92568585219105015"/>
           <c:h val="0.70501341894454117"/>
         </c:manualLayout>
       </c:layout>
@@ -901,7 +941,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BurndownChart2-Sprint2'!$E$12</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -912,39 +952,48 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'BurndownChart2-Sprint2'!$I$1:$O$1</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$I$1:$M$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Start</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.10.2014</c:v>
+                  <c:v>27.11.2014</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>06.11.2014</c:v>
+                  <c:v>04.12.2014</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.11.2014</c:v>
+                  <c:v>11.12.2014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.11.2014</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27.11.2014</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>04.12.2014</c:v>
+                  <c:v>18.12.2014</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BurndownChart2-Sprint2'!$I$12:$O$12</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$I$8:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7050</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -955,7 +1004,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BurndownChart2-Sprint2'!$E$13</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$E$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -964,12 +1013,38 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'BurndownChart2-Sprint2'!$I$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.11.2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>04.12.2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.12.2014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.12.2014</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BurndownChart2-Sprint2'!$I$13:$O$13</c:f>
+              <c:f>'BurndownChart2-Sprint2'!$I$9:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9400</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -985,21 +1060,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92194304"/>
-        <c:axId val="102580800"/>
+        <c:axId val="126989312"/>
+        <c:axId val="125653504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92194304"/>
+        <c:axId val="126989312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102580800"/>
+        <c:crossAx val="125653504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1007,7 +1082,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102580800"/>
+        <c:axId val="125653504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,13 +1092,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="92194304"/>
+        <c:crossAx val="126989312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1081,13 +1157,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>98050</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>139513</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1401,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,38 +1492,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
+      <c r="A1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1456,15 +1532,15 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1473,15 +1549,15 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1493,7 +1569,7 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1532,271 +1608,271 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="F11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="H11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="I11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="18" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="E12" s="15"/>
+      <c r="F12" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
-      <c r="C12" s="21" t="s">
+      <c r="H12" s="15"/>
+      <c r="I12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21" t="s">
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="17">
         <v>34</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="22">
-        <v>34</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="22">
+      <c r="C13" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="17">
         <v>1</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="22">
+      <c r="F13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="17">
         <v>55</v>
       </c>
-      <c r="I13" s="23" t="s">
-        <v>70</v>
+      <c r="I13" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="F15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="H15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="I15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="18" t="s">
+    </row>
+    <row r="16" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
-      <c r="C16" s="21" t="s">
+      <c r="H16" s="15"/>
+      <c r="I16" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="22">
+      <c r="B17" s="17">
         <v>21</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="17">
+        <v>34</v>
+      </c>
+      <c r="I17" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="E17" s="22">
-        <v>2</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="22">
-        <v>34</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="F19" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="H19" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="I19" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="18" t="s">
+    </row>
+    <row r="20" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="E20" s="15"/>
+      <c r="F20" s="16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="21" t="s">
+      <c r="H20" s="15"/>
+      <c r="I20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22">
+      <c r="B21" s="17">
         <v>21</v>
       </c>
-      <c r="C21" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="22">
+      <c r="C21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="17">
         <v>89</v>
       </c>
-      <c r="F21" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" s="22">
+      <c r="F21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="17">
         <v>13</v>
       </c>
-      <c r="I21" s="23" t="s">
-        <v>73</v>
+      <c r="I21" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="F23" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="H23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="I23" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="18" t="s">
+    </row>
+    <row r="24" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="E24" s="15"/>
+      <c r="F24" s="16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="21" t="s">
+      <c r="H24" s="15"/>
+      <c r="I24" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="21" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22">
+      <c r="B25" s="17">
         <v>34</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="22">
+      <c r="C25" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="17">
         <v>55</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" s="22">
+      <c r="F25" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="17">
         <v>34</v>
       </c>
-      <c r="I25" s="23" t="s">
-        <v>73</v>
+      <c r="I25" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:9" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="19" t="s">
+      <c r="B27" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="H27" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15"/>
+      <c r="C28" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="I27" s="19"/>
-    </row>
-    <row r="28" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="C28" s="21" t="s">
+      <c r="H28" s="15"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="17">
+        <v>21</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="21"/>
-    </row>
-    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="22">
-        <v>21</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="22">
+      <c r="E29" s="17">
         <v>34</v>
       </c>
-      <c r="F29" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23" t="s">
-        <v>36</v>
+      <c r="F29" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1813,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1827,98 +1903,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="E1" s="24" t="s">
+      <c r="A1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="10">
+      <c r="J1" s="7">
         <v>41949</v>
       </c>
-      <c r="K1" s="10">
+      <c r="K1" s="7">
         <v>41956</v>
       </c>
-      <c r="L1" s="10">
+      <c r="L1" s="7">
         <v>41963</v>
       </c>
-      <c r="M1" s="10">
+      <c r="M1" s="32">
         <v>41970</v>
       </c>
-      <c r="N1" s="11">
-        <v>41977</v>
-      </c>
-      <c r="O1" s="11">
-        <v>41984</v>
-      </c>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2100</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D3" s="3"/>
+      <c r="E3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F3" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3">
-        <v>34</v>
-      </c>
-      <c r="H2" s="3">
-        <v>2100</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D3" s="4"/>
-      <c r="E3" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>500</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
-        <v>77</v>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1927,31 +1999,31 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="D4" s="25"/>
+      <c r="E4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2">
         <v>55</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>2100</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
-        <v>77</v>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="4"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1960,31 +2032,31 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="D5" s="25"/>
+      <c r="E5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2">
         <v>21</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>2100</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>77</v>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="4"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1996,26 +2068,26 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="D6" s="3"/>
+      <c r="E6" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>500</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="4"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -2027,26 +2099,26 @@
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="D7" s="3"/>
+      <c r="E7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="2">
         <v>34</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>2100</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="4"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -2058,89 +2130,89 @@
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="25" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="2">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2100</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D9" s="3"/>
+      <c r="E9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F9" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="3">
-        <v>21</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G9" s="2">
+        <v>89</v>
+      </c>
+      <c r="H9" s="2">
         <v>2100</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D9" s="4"/>
-      <c r="E9" s="25" t="s">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F10" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="3">
-        <v>89</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2100</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>13</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>1300</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
-        <v>77</v>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="4"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="E11" s="32" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="E11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="1">
         <f>SUM(H2:H10)</f>
         <v>14900</v>
@@ -2149,89 +2221,86 @@
         <v>14900</v>
       </c>
       <c r="J11" s="1">
-        <f>14900-2483.33333333333</f>
-        <v>12416.66666666667</v>
-      </c>
-      <c r="K11" s="3">
-        <v>9933.3333333332994</v>
-      </c>
-      <c r="L11" s="3">
+        <v>11175</v>
+      </c>
+      <c r="K11" s="2">
         <v>7450</v>
       </c>
-      <c r="M11" s="1">
-        <v>4966.6666666666597</v>
-      </c>
-      <c r="N11" s="1">
-        <v>2483.3333333333298</v>
-      </c>
-      <c r="O11" s="4">
+      <c r="L11" s="2">
+        <v>3725</v>
+      </c>
+      <c r="M11" s="3">
         <v>0</v>
       </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5">
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
         <v>14900</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <f>I11-H3</f>
         <v>14400</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="4">
         <v>14400</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <f>6300-2100</f>
         <v>4200</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
+      <c r="M12" s="5">
+        <v>4200</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H14" s="1">
         <f>SUM(G2:G10)</f>
         <v>270</v>
       </c>
-      <c r="I14" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="3">
+      <c r="I14" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="2">
         <f>SUM(H11)</f>
         <v>14900</v>
       </c>
-      <c r="K14" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="L14" s="3">
+      <c r="K14" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="2">
         <f>J14/H14</f>
         <v>55.185185185185183</v>
       </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
+      <c r="A36" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2251,145 +2320,163 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:C35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="58" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="58" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="8" t="s">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="10">
-        <v>41942</v>
-      </c>
-      <c r="K1" s="10">
-        <v>41949</v>
-      </c>
-      <c r="L1" s="10">
-        <v>41956</v>
-      </c>
-      <c r="M1" s="10">
-        <v>41963</v>
-      </c>
-      <c r="N1" s="10">
+      <c r="J1" s="7">
         <v>41970</v>
       </c>
-      <c r="O1" s="11">
+      <c r="K1" s="7">
         <v>41977</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="L1" s="7">
+        <v>41984</v>
+      </c>
+      <c r="M1" s="32">
+        <v>41991</v>
+      </c>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+      <c r="E2" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2">
+        <v>500</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D3" s="3"/>
+      <c r="E3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
+        <v>2100</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D4" s="25"/>
+      <c r="E4" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>2100</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D5" s="25"/>
+      <c r="E5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>1300</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2399,20 +2486,26 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>2100</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2422,20 +2515,26 @@
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>1300</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2445,128 +2544,150 @@
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="32" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="34" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="1">
+        <f>SUM(H2:H7)</f>
+        <v>9400</v>
+      </c>
+      <c r="I8" s="1">
+        <v>9400</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7050</v>
+      </c>
+      <c r="K8" s="2">
+        <v>4700</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2350</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D9" s="3"/>
+      <c r="E9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4">
+        <v>9400</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="1">
+        <f>SUM(G2:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9400</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="2" t="e">
+        <f>J11/H11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="38"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A35:C35"/>
+  <mergeCells count="9">
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A10:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAJ Documents après rétro.
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -531,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -578,27 +578,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -613,13 +597,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,11 +820,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126554112"/>
-        <c:axId val="95000768"/>
+        <c:axId val="126234624"/>
+        <c:axId val="89757888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126554112"/>
+        <c:axId val="126234624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +834,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95000768"/>
+        <c:crossAx val="89757888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -848,7 +842,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95000768"/>
+        <c:axId val="89757888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,7 +852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="126554112"/>
+        <c:crossAx val="126234624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1060,11 +1054,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126989312"/>
-        <c:axId val="125653504"/>
+        <c:axId val="92132864"/>
+        <c:axId val="126304832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126989312"/>
+        <c:axId val="92132864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1068,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125653504"/>
+        <c:crossAx val="126304832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1082,7 +1076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125653504"/>
+        <c:axId val="126304832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1086,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="126989312"/>
+        <c:crossAx val="92132864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1492,11 +1486,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1890,7 +1884,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1903,11 +1897,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
       <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
@@ -1932,11 +1926,11 @@
       <c r="L1" s="7">
         <v>41963</v>
       </c>
-      <c r="M1" s="32">
+      <c r="M1" s="23">
         <v>41970</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -1949,7 +1943,7 @@
       <c r="E2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="25" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="2">
@@ -1973,7 +1967,7 @@
       <c r="E3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="26" t="s">
         <v>28</v>
       </c>
       <c r="G3" s="2">
@@ -1999,14 +1993,14 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="26" t="s">
         <v>30</v>
       </c>
       <c r="G4" s="2">
@@ -2032,14 +2026,14 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="2">
@@ -2072,7 +2066,7 @@
       <c r="E6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="26" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="2">
@@ -2103,7 +2097,7 @@
       <c r="E7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="26" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="2">
@@ -2134,7 +2128,7 @@
       <c r="E8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="26" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="2">
@@ -2156,7 +2150,7 @@
       <c r="E9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="26" t="s">
         <v>47</v>
       </c>
       <c r="G9" s="2">
@@ -2176,16 +2170,16 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="3"/>
       <c r="E10" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="26" t="s">
         <v>49</v>
       </c>
       <c r="G10" s="2">
@@ -2205,14 +2199,14 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="E11" s="26" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="E11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="1">
         <f>SUM(H2:H10)</f>
         <v>14900</v>
@@ -2236,11 +2230,11 @@
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4">
         <v>14900</v>
@@ -2296,11 +2290,11 @@
       <c r="O14" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="23"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2323,7 +2317,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2337,11 +2331,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
       <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
@@ -2366,11 +2360,11 @@
       <c r="L1" s="7">
         <v>41984</v>
       </c>
-      <c r="M1" s="32">
+      <c r="M1" s="23">
         <v>41991</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -2383,10 +2377,12 @@
       <c r="E2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
       <c r="H2" s="2">
         <v>500</v>
       </c>
@@ -2403,10 +2399,12 @@
       <c r="E3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2">
+        <v>13</v>
+      </c>
       <c r="H3" s="2">
         <v>2100</v>
       </c>
@@ -2425,17 +2423,19 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>8</v>
+      </c>
       <c r="H4" s="2">
         <v>2100</v>
       </c>
@@ -2454,17 +2454,19 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>13</v>
+      </c>
       <c r="H5" s="2">
         <v>1300</v>
       </c>
@@ -2490,10 +2492,12 @@
       <c r="E6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>8</v>
+      </c>
       <c r="H6" s="2">
         <v>2100</v>
       </c>
@@ -2517,12 +2521,14 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="2">
+        <v>13</v>
+      </c>
       <c r="H7" s="2">
         <v>1300</v>
       </c>
@@ -2545,11 +2551,11 @@
         <v>10</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="1">
         <f>SUM(H2:H7)</f>
         <v>9400</v>
@@ -2574,11 +2580,11 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D9" s="3"/>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4">
         <v>9400</v>
@@ -2591,35 +2597,35 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="2"/>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
       <c r="H11" s="1">
         <f>SUM(G2:G10)</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>73</v>
@@ -2630,11 +2636,11 @@
       <c r="K11" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="2" t="e">
+      <c r="L11" s="2">
         <f>J11/H11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="38"/>
+        <v>167.85714285714286</v>
+      </c>
+      <c r="M11" s="28"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
@@ -2643,12 +2649,12 @@
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
@@ -2668,11 +2674,11 @@
       <c r="O14" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="23"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Documentations complétée et ajout de la rétro
</commit_message>
<xml_diff>
--- a/Documents/DocumentsGroupeC.xlsx
+++ b/Documents/DocumentsGroupeC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="90">
   <si>
     <t>Nom</t>
   </si>
@@ -543,19 +543,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -566,11 +553,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -626,9 +624,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -653,6 +648,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,11 +863,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106238464"/>
-        <c:axId val="87791808"/>
+        <c:axId val="42017280"/>
+        <c:axId val="90740928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106238464"/>
+        <c:axId val="42017280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +877,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87791808"/>
+        <c:crossAx val="90740928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -881,7 +885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87791808"/>
+        <c:axId val="90740928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="106238464"/>
+        <c:crossAx val="42017280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1081,6 +1085,15 @@
                 <c:pt idx="1">
                   <c:v>7300</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>7300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1300</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1096,11 +1109,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106241536"/>
-        <c:axId val="105988672"/>
+        <c:axId val="42018816"/>
+        <c:axId val="42091072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106241536"/>
+        <c:axId val="42018816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1123,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105988672"/>
+        <c:crossAx val="42091072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1118,7 +1131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105988672"/>
+        <c:axId val="42091072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="106241536"/>
+        <c:crossAx val="42018816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1513,7 +1526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -1528,11 +1541,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2060,11 +2073,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
       <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
@@ -2106,7 +2119,7 @@
       <c r="E2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="2">
@@ -2130,7 +2143,7 @@
       <c r="E3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="25" t="s">
         <v>28</v>
       </c>
       <c r="G3" s="2">
@@ -2156,14 +2169,14 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G4" s="2">
@@ -2189,14 +2202,14 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="2">
@@ -2229,7 +2242,7 @@
       <c r="E6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="2">
@@ -2260,7 +2273,7 @@
       <c r="E7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>39</v>
       </c>
       <c r="G7" s="2">
@@ -2291,7 +2304,7 @@
       <c r="E8" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>44</v>
       </c>
       <c r="G8" s="2">
@@ -2313,7 +2326,7 @@
       <c r="E9" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>46</v>
       </c>
       <c r="G9" s="2">
@@ -2333,16 +2346,16 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="3"/>
       <c r="E10" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="25" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="2">
@@ -2362,14 +2375,14 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="E11" s="34" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="E11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="1">
         <f>SUM(H2:H10)</f>
         <v>14900</v>
@@ -2393,11 +2406,11 @@
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4">
         <v>14900</v>
@@ -2453,11 +2466,11 @@
       <c r="O14" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2480,7 +2493,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2494,11 +2507,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
       <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
@@ -2537,10 +2550,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="2">
@@ -2550,7 +2563,9 @@
         <v>500</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="3"/>
@@ -2559,10 +2574,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D3" s="3"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="25" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="2">
@@ -2572,7 +2587,9 @@
         <v>2100</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="3"/>
@@ -2586,14 +2603,14 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="2">
@@ -2603,7 +2620,9 @@
         <v>2100</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="3"/>
@@ -2617,14 +2636,14 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>53</v>
       </c>
       <c r="G5" s="2">
@@ -2652,10 +2671,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="2">
@@ -2685,10 +2704,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="39" t="s">
         <v>64</v>
       </c>
       <c r="G7" s="2">
@@ -2698,7 +2717,9 @@
         <v>1300</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="3"/>
@@ -2716,11 +2737,11 @@
         <v>10</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="1">
         <f>SUM(H2:H7)</f>
         <v>9400</v>
@@ -2745,11 +2766,11 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D9" s="3"/>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4">
         <v>9400</v>
@@ -2758,39 +2779,46 @@
         <f>I9-H6</f>
         <v>7300</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
+      <c r="K9" s="4">
+        <v>7300</v>
+      </c>
+      <c r="L9" s="4">
+        <v>7300</v>
+      </c>
+      <c r="M9" s="5">
+        <f>3400-2100</f>
+        <v>1300</v>
+      </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="1">
         <f>SUM(G2:G10)</f>
         <v>56</v>
@@ -2808,21 +2836,21 @@
         <f>J11/H11</f>
         <v>167.85714285714286</v>
       </c>
-      <c r="M11" s="28"/>
+      <c r="M11" s="27"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D12" s="2"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
@@ -2842,11 +2870,11 @@
       <c r="O14" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>